<commit_message>
quiz done(without timer) and teacher can see quiz scores and whole report on quiz answeres for particular student
</commit_message>
<xml_diff>
--- a/media/quizzes/Django_Final_Exam.xlsx
+++ b/media/quizzes/Django_Final_Exam.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\omarh\OneDrive\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C41B35B-EF14-4CD9-9893-45C7CA262BEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3843B7B2-F7F4-4827-91F5-F3ADCB5C5420}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{08B05A73-B457-432E-8333-052C715F4391}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
   <si>
     <t>Question ID</t>
   </si>
@@ -91,9 +91,6 @@
   </si>
   <si>
     <t xml:space="preserve"> By default, Django configuration uses SQLight database?</t>
-  </si>
-  <si>
-    <t>Django is written in C++?</t>
   </si>
 </sst>
 </file>
@@ -140,16 +137,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </left>
       <right style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </right>
       <top style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -157,8 +154,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -485,7 +488,7 @@
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -500,141 +503,127 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="24" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="2">
+      <c r="A2" s="4">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="I2" s="2">
-        <v>2</v>
+      <c r="I2" s="4">
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="22.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="2">
+      <c r="A3" s="4">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="2" t="b">
+      <c r="D3" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="E3" s="2" t="b">
+      <c r="E3" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="F3" s="2" t="b">
+      <c r="F3" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="2">
-        <v>1</v>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="4">
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="2">
+      <c r="A4" s="4">
         <v>3</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G4" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="H4" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="I4" s="2">
-        <v>2</v>
+      <c r="I4" s="4">
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="2">
-        <v>4</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E5" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F5" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="2">
-        <v>1</v>
-      </c>
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>